<commit_message>
minor adjustments to emx
</commit_message>
<xml_diff>
--- a/dist/rd3_portal_cluster.xlsx
+++ b/dist/rd3_portal_cluster.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="106">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -48,9 +48,18 @@
     <t>freeze1</t>
   </si>
   <si>
+    <t>freeze1-patch1</t>
+  </si>
+  <si>
+    <t>freeze1-patch3</t>
+  </si>
+  <si>
     <t>freeze2</t>
   </si>
   <si>
+    <t>freeze2-patch1</t>
+  </si>
+  <si>
     <t>freeze3</t>
   </si>
   <si>
@@ -63,9 +72,21 @@
     <t>Freeze 1 Files</t>
   </si>
   <si>
+    <t>Freeze 1 Patch 1 Files</t>
+  </si>
+  <si>
+    <t>Freeze 1 Patch 3 Files</t>
+  </si>
+  <si>
     <t>Freeze 2 Files</t>
   </si>
   <si>
+    <t>Freeze 2 Patch 1 Files</t>
+  </si>
+  <si>
+    <t>Freeze 3 Files</t>
+  </si>
+  <si>
     <t>Extracted data from Phenopacket files</t>
   </si>
   <si>
@@ -73,6 +94,12 @@
   </si>
   <si>
     <t>attribute template for listing all files of a release or type</t>
+  </si>
+  <si>
+    <t>Original gvcf, bam, ped, phenopacket</t>
+  </si>
+  <si>
+    <t>Updated ped and phenopacket files</t>
   </si>
   <si>
     <t>rd3_portal_cluster_template</t>
@@ -661,16 +688,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -705,7 +732,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -713,22 +740,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -739,10 +766,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -753,10 +780,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -767,7 +794,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -781,10 +808,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -795,10 +825,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -809,10 +842,64 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -830,45 +917,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -877,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -888,16 +975,16 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -908,16 +995,16 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -928,16 +1015,16 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -948,16 +1035,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -968,16 +1055,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -988,16 +1075,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -1008,16 +1095,16 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -1028,16 +1115,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -1048,16 +1135,16 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -1071,16 +1158,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -1091,16 +1178,16 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -1111,16 +1198,16 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -1131,16 +1218,16 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -1151,16 +1238,16 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -1174,13 +1261,13 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1189,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -1203,16 +1290,16 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -1223,16 +1310,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -1243,16 +1330,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -1263,16 +1350,16 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -1283,16 +1370,16 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -1303,16 +1390,16 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
@@ -1323,16 +1410,16 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
@@ -1343,16 +1430,16 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
@@ -1363,16 +1450,16 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1383,16 +1470,16 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F27" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -1403,16 +1490,16 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F28" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -1423,16 +1510,16 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F29" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1443,16 +1530,16 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -1466,16 +1553,16 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -1486,16 +1573,16 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -1506,16 +1593,16 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -1529,16 +1616,16 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
@@ -1549,13 +1636,13 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F35" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
@@ -1566,13 +1653,13 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F36" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -1583,13 +1670,13 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1600,13 +1687,13 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F38" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -1617,13 +1704,13 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G39" t="b">
         <v>1</v>
@@ -1634,13 +1721,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F40" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -1651,13 +1738,13 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F41" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G41" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
minor fixes to PED data staging table
</commit_message>
<xml_diff>
--- a/dist/rd3_portal_cluster.xlsx
+++ b/dist/rd3_portal_cluster.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="105">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -30,10 +30,10 @@
     <t>Cluster Data</t>
   </si>
   <si>
-    <t>RD3 portal, containing data submitted by CNAG (v1.1.0, 2021-10-11)</t>
-  </si>
-  <si>
-    <t>Extracted metadata PED and Phenopacket files stored on the cluster (v1.1.0, 2022-09-01)</t>
+    <t>RD3 portal, containing data submitted by CNAG(v1.1.0, 2021-10-11)</t>
+  </si>
+  <si>
+    <t>Extracted metadata PED and Phenopacket files stored on the cluster(v1.1.0, 2022-09-01)</t>
   </si>
   <si>
     <t>phenopacket</t>
@@ -156,7 +156,7 @@
     <t>processed</t>
   </si>
   <si>
-    <t>rowID</t>
+    <t>id</t>
   </si>
   <si>
     <t>pedID</t>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>defaultValue</t>
-  </si>
-  <si>
-    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -909,13 +906,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -943,11 +940,8 @@
       <c r="I1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -973,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -993,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1013,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1033,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1053,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1073,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1093,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1113,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1133,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1156,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1176,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1196,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1216,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1236,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1259,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1284,11 +1278,8 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-      <c r="J17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1328,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1348,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1368,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1388,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1408,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1428,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1448,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1468,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1488,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1508,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1528,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1551,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1571,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>30</v>
       </c>

</xml_diff>